<commit_message>
Dodani podatki o podjetjih
https://github.com/masbug/etoro-edavki/issues/36#issuecomment-1951471612
</commit_message>
<xml_diff>
--- a/Company_info.xlsx
+++ b/Company_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Dev\eDavki\etoro-edavki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658D9168-5754-435F-914F-68235BCFC4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910D3D61-9C81-425C-BCEF-F23167EAF1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="1396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="1524">
   <si>
     <t>Symbol</t>
   </si>
@@ -4208,13 +4208,397 @@
   </si>
   <si>
     <t>55 East 52nd Street, New York, NY 10055, United States</t>
+  </si>
+  <si>
+    <t>AGR.US</t>
+  </si>
+  <si>
+    <t>US05351W1036</t>
+  </si>
+  <si>
+    <t>Avangrid Inc</t>
+  </si>
+  <si>
+    <t>180 Marsh Hill Road, Orange, CT 06477, USA</t>
+  </si>
+  <si>
+    <t>QYLD</t>
+  </si>
+  <si>
+    <t>US37954Y4834</t>
+  </si>
+  <si>
+    <t>Global X Nasdaq 100 Covered Call ETF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirae Asset Global Investments Co., Ltd., 625 Madison Avenue, 3rd Floor New York, NY 10022 </t>
+  </si>
+  <si>
+    <t>IBE</t>
+  </si>
+  <si>
+    <t>ES0144580Y14</t>
+  </si>
+  <si>
+    <t>Iberdrola</t>
+  </si>
+  <si>
+    <t>PL EUSKADI 5, 48008 BILBAO, Spain</t>
+  </si>
+  <si>
+    <t>AQN</t>
+  </si>
+  <si>
+    <t>CA0158571053</t>
+  </si>
+  <si>
+    <t>Algonquin Power &amp; Utilities Corp</t>
+  </si>
+  <si>
+    <t>354 Davis Road, Suite 100, Oakville, ON L6J 2X1, Canada</t>
+  </si>
+  <si>
+    <t>SPHD</t>
+  </si>
+  <si>
+    <t>US46138E3624</t>
+  </si>
+  <si>
+    <t>Invesco S&amp;P 500 High Dividend Low Volatility ETF</t>
+  </si>
+  <si>
+    <t>Invesco Ltd., Two Peachtree Pointe, 1555 Peachtree Street, N.E., Suite 1800, Atlanta, Georgia 30309</t>
+  </si>
+  <si>
+    <t>SHY</t>
+  </si>
+  <si>
+    <t>US4642874576</t>
+  </si>
+  <si>
+    <t>iShares 1-3 Year Treasury Bond ETF</t>
+  </si>
+  <si>
+    <t>BlackRock Fund Advisors, 400 Howard Street, San Francisco, CA 94105, USA</t>
+  </si>
+  <si>
+    <t>IEF</t>
+  </si>
+  <si>
+    <t>US4642874402</t>
+  </si>
+  <si>
+    <t>iShares 7-10 Year Treasury Bond ETF</t>
+  </si>
+  <si>
+    <t>SDIV</t>
+  </si>
+  <si>
+    <t>US37960A6698</t>
+  </si>
+  <si>
+    <t>Global X SuperDividend ETF</t>
+  </si>
+  <si>
+    <t>LNT</t>
+  </si>
+  <si>
+    <t>US0188021085</t>
+  </si>
+  <si>
+    <t>Alliant Energy Corp</t>
+  </si>
+  <si>
+    <t>4902 North Biltmore Lane, 53718 Madison, WI, USA</t>
+  </si>
+  <si>
+    <t>SSE.L</t>
+  </si>
+  <si>
+    <t>GB0007908733</t>
+  </si>
+  <si>
+    <t>SSE</t>
+  </si>
+  <si>
+    <t>SSE plc, Inveralmond House, 200 Dunkeld Road, Perth PH1 3AQ, United Kingdom</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>US5184391044</t>
+  </si>
+  <si>
+    <t>Estee Lauder Companies Inc</t>
+  </si>
+  <si>
+    <t>767 Fifth Avenue, New York, NY 10153, United States</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>US2091151041</t>
+  </si>
+  <si>
+    <t>Consolidated Edison Inc</t>
+  </si>
+  <si>
+    <t>4 Irving Place, New York, New York 10003, USA</t>
+  </si>
+  <si>
+    <t>VEU</t>
+  </si>
+  <si>
+    <t>US9220427754</t>
+  </si>
+  <si>
+    <t>Vanguard FTSE All-World ex-US</t>
+  </si>
+  <si>
+    <t>The Vanguard Group Instl, P.O. Box 2900 Valley Forge, PA 19482-2900 USA</t>
+  </si>
+  <si>
+    <t>ORA.US</t>
+  </si>
+  <si>
+    <t>US6866881021</t>
+  </si>
+  <si>
+    <t>Ormat Technologies Inc.</t>
+  </si>
+  <si>
+    <t>6140 Plumas Street, Reno, NV 89519-6075, USA</t>
+  </si>
+  <si>
+    <t>VTV</t>
+  </si>
+  <si>
+    <t>US9229087443</t>
+  </si>
+  <si>
+    <t>Vanguard Value ETF</t>
+  </si>
+  <si>
+    <t>SCHD</t>
+  </si>
+  <si>
+    <t>US8085247976</t>
+  </si>
+  <si>
+    <t>Schwab US Dividend Equity ETF</t>
+  </si>
+  <si>
+    <t>Charles Schwab &amp; Co., Inc., 1360 3RD Ave FL 1 New York, NY, 10075-0461 USA</t>
+  </si>
+  <si>
+    <t>NOBL</t>
+  </si>
+  <si>
+    <t>US74348A4673</t>
+  </si>
+  <si>
+    <t>ProShares S&amp;P 500 Dividend Aristocrats ETF</t>
+  </si>
+  <si>
+    <t>ProShares, 7272 Wisconsin Ave. 21st Floor Bethesda, MD 20814</t>
+  </si>
+  <si>
+    <t>IJR</t>
+  </si>
+  <si>
+    <t>US4642878049</t>
+  </si>
+  <si>
+    <t>iShares Core S&amp;P Small-Cap ETF</t>
+  </si>
+  <si>
+    <t>VOOG</t>
+  </si>
+  <si>
+    <t>US9219325050</t>
+  </si>
+  <si>
+    <t>Vanguard S&amp;P 500 Growth ETF</t>
+  </si>
+  <si>
+    <t>VFH</t>
+  </si>
+  <si>
+    <t>US92204A4058</t>
+  </si>
+  <si>
+    <t>Vanguard Financials ETF</t>
+  </si>
+  <si>
+    <t>AY</t>
+  </si>
+  <si>
+    <t>GB00BLP5YB54</t>
+  </si>
+  <si>
+    <t>Atlantica Sustainable Infrastructure PLC</t>
+  </si>
+  <si>
+    <t>Great West House, GW1 17th Floor Great West Road, Brentford TW8 9DF, United Kingdom</t>
+  </si>
+  <si>
+    <t>LQDE</t>
+  </si>
+  <si>
+    <t>IE0032895942</t>
+  </si>
+  <si>
+    <t>iShares $ Corporate Bond UCITS ETF</t>
+  </si>
+  <si>
+    <t>EDP.LSB</t>
+  </si>
+  <si>
+    <t>PTEDP0AM0009</t>
+  </si>
+  <si>
+    <t>EDP - Energias de Portugal SA</t>
+  </si>
+  <si>
+    <t>Avenida 24 de Julho 12, 4th Floor, Lisbon 1249-300, Portugal</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>ENGI</t>
+  </si>
+  <si>
+    <t>FR0010208488</t>
+  </si>
+  <si>
+    <t>Engie SA</t>
+  </si>
+  <si>
+    <t>1, place Samuel de Champlain, Courbevoie 92400, France</t>
+  </si>
+  <si>
+    <t>RWE.DE</t>
+  </si>
+  <si>
+    <t>DE0007037129</t>
+  </si>
+  <si>
+    <t>RWE AG</t>
+  </si>
+  <si>
+    <t>RWE Platz 1-7, 45141 Essen, Deutschland</t>
+  </si>
+  <si>
+    <t>NIBEB.ST</t>
+  </si>
+  <si>
+    <t>SE0015988019</t>
+  </si>
+  <si>
+    <t>Nibe Industrier AB Ser. B</t>
+  </si>
+  <si>
+    <t>Järnvägsgatan 40, Markaryd 285 32, Sweden</t>
+  </si>
+  <si>
+    <t>RSP</t>
+  </si>
+  <si>
+    <t>US46137V3574</t>
+  </si>
+  <si>
+    <t>Invesco S&amp;P 500 Equal Weight ETF</t>
+  </si>
+  <si>
+    <t>XLP</t>
+  </si>
+  <si>
+    <t>US81369Y3080</t>
+  </si>
+  <si>
+    <t>Consumer Staples Select Sector SPDR</t>
+  </si>
+  <si>
+    <t>SQQQ</t>
+  </si>
+  <si>
+    <t>US74347G4322</t>
+  </si>
+  <si>
+    <t>ProShares UltraPro Short QQQ</t>
+  </si>
+  <si>
+    <t>SRTY</t>
+  </si>
+  <si>
+    <t>US74347G3902</t>
+  </si>
+  <si>
+    <t>ProShares UltraPro Short Russell2000</t>
+  </si>
+  <si>
+    <t>TMF</t>
+  </si>
+  <si>
+    <t>US25460G1388</t>
+  </si>
+  <si>
+    <t>Direxion Daily 20 Year Plus Treasury Bull 3x Shares</t>
+  </si>
+  <si>
+    <t>3800.HK</t>
+  </si>
+  <si>
+    <t>KYG3774X1088</t>
+  </si>
+  <si>
+    <t>GCL Technology Holdings Ltd</t>
+  </si>
+  <si>
+    <t>International Commerce Centre, Level 17 Unit 1703B-1706 1 Austin Road West, Kowloon, Hong Kong</t>
+  </si>
+  <si>
+    <t>ANA</t>
+  </si>
+  <si>
+    <t>ES0125220311</t>
+  </si>
+  <si>
+    <t>Acciona</t>
+  </si>
+  <si>
+    <t>Avenida de Europa, 18, Parque Empresarial La Moraleja, Alcobendas 28108, Spain</t>
+  </si>
+  <si>
+    <t>0916.HK</t>
+  </si>
+  <si>
+    <t>CNE100000HD4</t>
+  </si>
+  <si>
+    <t>China Longyuan</t>
+  </si>
+  <si>
+    <t>Block C, 6-9 Fuchengmen North Street Bejing, China, 100034</t>
+  </si>
+  <si>
+    <t>TAN</t>
+  </si>
+  <si>
+    <t>US46138G7060</t>
+  </si>
+  <si>
+    <t>Invesco Solar ETF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4225,10 +4609,23 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -4250,21 +4647,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Navadno" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Navadno 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Navadno 2 2" xfId="2" xr:uid="{A6128BC9-A440-44F0-B407-83B01CC70D87}"/>
+    <cellStyle name="Navadno 3" xfId="3" xr:uid="{78F38918-51BC-4D42-8584-4E63912D672B}"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -4314,7 +4717,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E348" headerRowCellStyle="Navadno" dataCellStyle="Navadno" totalsRowCellStyle="Navadno">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E383" headerRowCellStyle="Navadno" dataCellStyle="Navadno" totalsRowCellStyle="Navadno">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Symbol" dataCellStyle="Navadno"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ISIN" dataCellStyle="Navadno"/>
@@ -4526,8 +4929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E962"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
-      <selection activeCell="D158" sqref="D158"/>
+    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
+      <selection activeCell="B383" sqref="B383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10457,42 +10860,602 @@
         <v>146</v>
       </c>
     </row>
-    <row r="349" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B349" s="2" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C349" s="2" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D349" s="2" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E349" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A350" s="2" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B350" s="2" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C350" s="2" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D350" s="2" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E350" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A351" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B351" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C351" s="2" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D351" s="2" t="s">
+        <v>1407</v>
+      </c>
+      <c r="E351" s="3" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A352" s="2" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B352" s="2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C352" s="2" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D352" s="2" t="s">
+        <v>1411</v>
+      </c>
+      <c r="E352" s="3" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="2" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B353" s="2" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C353" s="2" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D353" s="2" t="s">
+        <v>1415</v>
+      </c>
+      <c r="E353" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A354" s="2" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B354" s="2" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C354" s="2" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D354" s="2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E354" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A355" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B355" s="2" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C355" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D355" s="2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E355" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A356" s="2" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B356" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D356" s="2" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E356" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A357" s="2" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B357" s="2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D357" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E357" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A358" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B358" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D358" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E358" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A359" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B359" s="2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D359" s="2" t="s">
+        <v>1437</v>
+      </c>
+      <c r="E359" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A360" s="2" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B360" s="2" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C360" s="2" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D360" s="2" t="s">
+        <v>1441</v>
+      </c>
+      <c r="E360" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A361" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B361" s="2" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D361" s="2" t="s">
+        <v>1445</v>
+      </c>
+      <c r="E361" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="2" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B362" s="2" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C362" s="2" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D362" s="2" t="s">
+        <v>1449</v>
+      </c>
+      <c r="E362" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A363" s="2" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B363" s="2" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C363" s="2" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D363" s="2" t="s">
+        <v>1445</v>
+      </c>
+      <c r="E363" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A364" s="2" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B364" s="2" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C364" s="2" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D364" s="2" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E364" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A365" s="2" t="s">
+        <v>1457</v>
+      </c>
+      <c r="B365" s="2" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C365" s="2" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D365" s="2" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E365" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A366" s="2" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B366" s="2" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C366" s="2" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D366" s="2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E366" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A367" s="2" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B367" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C367" s="2" t="s">
+        <v>1466</v>
+      </c>
+      <c r="D367" s="2" t="s">
+        <v>1445</v>
+      </c>
+      <c r="E367" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A368" s="2" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B368" s="2" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>1445</v>
+      </c>
+      <c r="E368" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="369" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A369" s="2" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B369" s="2" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D369" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E369" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A370" s="2" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B370" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E370" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="371" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A371" s="2" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B371" s="2" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D371" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="E371" s="3" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="372" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A372" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B372" s="2" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>1484</v>
+      </c>
+      <c r="D372" s="2" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E372" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="373" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A373" s="2" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B373" s="2" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D373" s="2" t="s">
+        <v>1489</v>
+      </c>
+      <c r="E373" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="374" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A374" s="2" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B374" s="2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>1493</v>
+      </c>
+      <c r="E374" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="375" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A375" s="2" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B375" s="2" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D375" s="2" t="s">
+        <v>1415</v>
+      </c>
+      <c r="E375" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="376" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A376" s="2" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B376" s="2" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C376" s="2" t="s">
+        <v>1499</v>
+      </c>
+      <c r="D376" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="E376" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="377" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A377" s="2" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B377" s="2" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C377" s="2" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D377" s="2" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E377" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="378" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A378" s="2" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B378" s="2" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C378" s="2" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D378" s="2" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E378" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A379" s="2" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B379" s="2" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C379" s="2" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D379" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="E379" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A380" s="2" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B380" s="2" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C380" s="2" t="s">
+        <v>1511</v>
+      </c>
+      <c r="D380" s="2" t="s">
+        <v>1512</v>
+      </c>
+      <c r="E380" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="381" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A381" s="2" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B381" s="2" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C381" s="2" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D381" s="2" t="s">
+        <v>1516</v>
+      </c>
+      <c r="E381" s="3" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A382" s="2" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C382" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D382" s="2" t="s">
+        <v>1520</v>
+      </c>
+      <c r="E382" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="383" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A383" s="2" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B383" s="2" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="D383" s="2" t="s">
+        <v>1415</v>
+      </c>
+      <c r="E383" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="384" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11072,6 +12035,7 @@
     <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>